<commit_message>
Comments and Deaths Model Filter >10
</commit_message>
<xml_diff>
--- a/2020-03-20-Germany-Covid19-Death-Prediction.xlsx
+++ b/2020-03-20-Germany-Covid19-Death-Prediction.xlsx
@@ -386,7 +386,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D25"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -405,302 +405,218 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="2">
-        <v>43899</v>
+        <v>43905</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="2">
-        <v>43900</v>
+        <v>43906</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>17</v>
       </c>
       <c r="D3">
-        <v>2</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="2">
-        <v>43901</v>
+        <v>43907</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="D4">
-        <v>3</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="2">
-        <v>43902</v>
+        <v>43908</v>
       </c>
       <c r="B5">
         <v>3</v>
       </c>
       <c r="C5">
-        <v>3</v>
+        <v>28</v>
       </c>
       <c r="D5">
-        <v>4</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="2">
-        <v>43903</v>
+        <v>43909</v>
       </c>
       <c r="B6">
         <v>4</v>
       </c>
       <c r="C6">
-        <v>7</v>
+        <v>44</v>
       </c>
       <c r="D6">
-        <v>5</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="2">
-        <v>43904</v>
+        <v>43910</v>
       </c>
       <c r="B7">
         <v>5</v>
       </c>
       <c r="C7">
-        <v>9</v>
+        <v>67</v>
       </c>
       <c r="D7">
-        <v>8</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="2">
-        <v>43905</v>
+        <v>43911</v>
       </c>
       <c r="B8">
         <v>6</v>
       </c>
-      <c r="C8">
-        <v>11</v>
-      </c>
       <c r="D8">
-        <v>11</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="2">
-        <v>43906</v>
+        <v>43912</v>
       </c>
       <c r="B9">
         <v>7</v>
       </c>
-      <c r="C9">
-        <v>17</v>
-      </c>
       <c r="D9">
-        <v>16</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="2">
-        <v>43907</v>
+        <v>43913</v>
       </c>
       <c r="B10">
         <v>8</v>
       </c>
-      <c r="C10">
-        <v>24</v>
-      </c>
       <c r="D10">
-        <v>22</v>
+        <v>177</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="2">
-        <v>43908</v>
+        <v>43914</v>
       </c>
       <c r="B11">
         <v>9</v>
       </c>
-      <c r="C11">
-        <v>28</v>
-      </c>
       <c r="D11">
-        <v>31</v>
+        <v>250</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="2">
-        <v>43909</v>
+        <v>43915</v>
       </c>
       <c r="B12">
         <v>10</v>
       </c>
-      <c r="C12">
-        <v>44</v>
-      </c>
       <c r="D12">
-        <v>44</v>
+        <v>353</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="2">
-        <v>43910</v>
+        <v>43916</v>
       </c>
       <c r="B13">
         <v>11</v>
       </c>
-      <c r="C13">
-        <v>67</v>
-      </c>
       <c r="D13">
-        <v>61</v>
+        <v>499</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="2">
-        <v>43911</v>
+        <v>43917</v>
       </c>
       <c r="B14">
         <v>12</v>
       </c>
       <c r="D14">
-        <v>86</v>
+        <v>703</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="2">
-        <v>43912</v>
+        <v>43918</v>
       </c>
       <c r="B15">
         <v>13</v>
       </c>
       <c r="D15">
-        <v>120</v>
+        <v>992</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="2">
-        <v>43913</v>
+        <v>43919</v>
       </c>
       <c r="B16">
         <v>14</v>
       </c>
       <c r="D16">
-        <v>167</v>
+        <v>1400</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="2">
-        <v>43914</v>
+        <v>43920</v>
       </c>
       <c r="B17">
         <v>15</v>
       </c>
       <c r="D17">
-        <v>233</v>
+        <v>1975</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="2">
-        <v>43915</v>
+        <v>43921</v>
       </c>
       <c r="B18">
         <v>16</v>
       </c>
       <c r="D18">
-        <v>326</v>
+        <v>2787</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="2">
-        <v>43916</v>
+        <v>43922</v>
       </c>
       <c r="B19">
         <v>17</v>
       </c>
       <c r="D19">
-        <v>455</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
-      <c r="A20" s="2">
-        <v>43917</v>
-      </c>
-      <c r="B20">
-        <v>18</v>
-      </c>
-      <c r="D20">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
-      <c r="A21" s="2">
-        <v>43918</v>
-      </c>
-      <c r="B21">
-        <v>19</v>
-      </c>
-      <c r="D21">
-        <v>887</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
-      <c r="A22" s="2">
-        <v>43919</v>
-      </c>
-      <c r="B22">
-        <v>20</v>
-      </c>
-      <c r="D22">
-        <v>1238</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
-      <c r="A23" s="2">
-        <v>43920</v>
-      </c>
-      <c r="B23">
-        <v>21</v>
-      </c>
-      <c r="D23">
-        <v>1728</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
-      <c r="A24" s="2">
-        <v>43921</v>
-      </c>
-      <c r="B24">
-        <v>22</v>
-      </c>
-      <c r="D24">
-        <v>2412</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
-      <c r="A25" s="2">
-        <v>43922</v>
-      </c>
-      <c r="B25">
-        <v>23</v>
-      </c>
-      <c r="D25">
-        <v>3367</v>
+        <v>3931</v>
       </c>
     </row>
   </sheetData>

</xml_diff>